<commit_message>
Fixed annotation and simplified repeated code
</commit_message>
<xml_diff>
--- a/Arduino-Leonardo/Saved-Data/HFP/HFP_TEST.xlsx
+++ b/Arduino-Leonardo/Saved-Data/HFP/HFP_TEST.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="359" uniqueCount="22">
   <si>
     <t>ParticipantCode</t>
   </si>
@@ -124,7 +124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -868,6 +868,266 @@
         <v>128</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2023</v>
+      </c>
+      <c r="E12" s="0">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0">
+        <v>30</v>
+      </c>
+      <c r="G12" s="0">
+        <v>15</v>
+      </c>
+      <c r="H12" s="0">
+        <v>23</v>
+      </c>
+      <c r="I12" s="0">
+        <v>30</v>
+      </c>
+      <c r="J12" s="0">
+        <v>200</v>
+      </c>
+      <c r="K12" s="0">
+        <v>25</v>
+      </c>
+      <c r="L12" s="0">
+        <v>125</v>
+      </c>
+      <c r="M12" s="0">
+        <v>65</v>
+      </c>
+      <c r="N12" s="0">
+        <v>65</v>
+      </c>
+      <c r="O12" s="0">
+        <v>65</v>
+      </c>
+      <c r="P12" s="0">
+        <v>113</v>
+      </c>
+      <c r="Q12" s="0">
+        <v>21</v>
+      </c>
+      <c r="R12" s="0">
+        <v>43</v>
+      </c>
+      <c r="S12" s="0">
+        <v>27</v>
+      </c>
+      <c r="T12" s="0">
+        <v>51</v>
+      </c>
+      <c r="U12" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0">
+        <v>2023</v>
+      </c>
+      <c r="E13" s="0">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0">
+        <v>30</v>
+      </c>
+      <c r="G13" s="0">
+        <v>15</v>
+      </c>
+      <c r="H13" s="0">
+        <v>23</v>
+      </c>
+      <c r="I13" s="0">
+        <v>40</v>
+      </c>
+      <c r="J13" s="0">
+        <v>250</v>
+      </c>
+      <c r="K13" s="0">
+        <v>250</v>
+      </c>
+      <c r="L13" s="0">
+        <v>250</v>
+      </c>
+      <c r="M13" s="0">
+        <v>250</v>
+      </c>
+      <c r="N13" s="0">
+        <v>250</v>
+      </c>
+      <c r="O13" s="0">
+        <v>250</v>
+      </c>
+      <c r="P13" s="0">
+        <v>250</v>
+      </c>
+      <c r="Q13" s="0">
+        <v>250</v>
+      </c>
+      <c r="R13" s="0">
+        <v>250</v>
+      </c>
+      <c r="S13" s="0">
+        <v>250</v>
+      </c>
+      <c r="T13" s="0">
+        <v>250</v>
+      </c>
+      <c r="U13" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0">
+        <v>3</v>
+      </c>
+      <c r="D14" s="0">
+        <v>2023</v>
+      </c>
+      <c r="E14" s="0">
+        <v>10</v>
+      </c>
+      <c r="F14" s="0">
+        <v>30</v>
+      </c>
+      <c r="G14" s="0">
+        <v>15</v>
+      </c>
+      <c r="H14" s="0">
+        <v>23</v>
+      </c>
+      <c r="I14" s="0">
+        <v>54</v>
+      </c>
+      <c r="J14" s="0">
+        <v>35</v>
+      </c>
+      <c r="K14" s="0">
+        <v>75</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0</v>
+      </c>
+      <c r="M14" s="0">
+        <v>0</v>
+      </c>
+      <c r="N14" s="0">
+        <v>0</v>
+      </c>
+      <c r="O14" s="0">
+        <v>14</v>
+      </c>
+      <c r="P14" s="0">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="0">
+        <v>14</v>
+      </c>
+      <c r="R14" s="0">
+        <v>14</v>
+      </c>
+      <c r="S14" s="0">
+        <v>14</v>
+      </c>
+      <c r="T14" s="0">
+        <v>14</v>
+      </c>
+      <c r="U14" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="0">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2023</v>
+      </c>
+      <c r="E15" s="0">
+        <v>10</v>
+      </c>
+      <c r="F15" s="0">
+        <v>30</v>
+      </c>
+      <c r="G15" s="0">
+        <v>15</v>
+      </c>
+      <c r="H15" s="0">
+        <v>43</v>
+      </c>
+      <c r="I15" s="0">
+        <v>16</v>
+      </c>
+      <c r="J15" s="0">
+        <v>52</v>
+      </c>
+      <c r="K15" s="0">
+        <v>52</v>
+      </c>
+      <c r="L15" s="0">
+        <v>50</v>
+      </c>
+      <c r="M15" s="0">
+        <v>30</v>
+      </c>
+      <c r="N15" s="0">
+        <v>0</v>
+      </c>
+      <c r="O15" s="0">
+        <v>10</v>
+      </c>
+      <c r="P15" s="0">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="0">
+        <v>10</v>
+      </c>
+      <c r="R15" s="0">
+        <v>16</v>
+      </c>
+      <c r="S15" s="0">
+        <v>16</v>
+      </c>
+      <c r="T15" s="0">
+        <v>13</v>
+      </c>
+      <c r="U15" s="0">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>